<commit_message>
added delay in Get_Flight_Info
</commit_message>
<xml_diff>
--- a/P2_Performer/Results/03-29-2023/Rich Drexel - Dallas, Texas, United States of America.xlsx
+++ b/P2_Performer/Results/03-29-2023/Rich Drexel - Dallas, Texas, United States of America.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\GetawayGurus\P2_Performer\Results\03-29-2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{52159366-3206-4070-BA0B-74CE03A5FBD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ABC10177-749C-421E-83F4-3B867BD808AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3108" yWindow="1848" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
   <si>
     <t>Hotel</t>
   </si>
@@ -146,19 +146,22 @@
     <t>Sonder at Commerce</t>
   </si>
   <si>
-    <t>Qatar AirwaysAmerican</t>
-  </si>
-  <si>
-    <t>9:05 AM – 10:00 AM+1</t>
-  </si>
-  <si>
-    <t>36 hr 55 min</t>
-  </si>
-  <si>
-    <t>6:45 PM – 9:35 AM+1</t>
-  </si>
-  <si>
-    <t>26 hr 50 min</t>
+    <t>Frontier</t>
+  </si>
+  <si>
+    <t>6:05 AM – 8:04 AM</t>
+  </si>
+  <si>
+    <t>2 hr 59 min</t>
+  </si>
+  <si>
+    <t>Spirit</t>
+  </si>
+  <si>
+    <t>11:10 AM – 1:03 PM</t>
+  </si>
+  <si>
+    <t>2 hr 53 min</t>
   </si>
   <si>
     <t>Renaissance Dallas Hotel</t>
@@ -1287,7 +1290,7 @@
     </row>
     <row r="4" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B4" s="63">
         <v>295</v>
@@ -1328,22 +1331,22 @@
         <v>38</v>
       </c>
       <c r="E6" s="60">
-        <v>1266</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B7" s="55" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C7" s="56"/>
       <c r="D7" s="14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E7" s="61">
-        <v>1386</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>